<commit_message>
feat: added flashcard content
</commit_message>
<xml_diff>
--- a/EuroSkills/Cisco/1001001001-ios.xlsx
+++ b/EuroSkills/Cisco/1001001001-ios.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Tasks" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelR1C1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="201">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -132,7 +132,7 @@
   </si>
   <si>
     <t xml:space="preserve">configure terminal
-  interface range {{ range }}
+  interface range {{ interface_range }}
     description NOT_USED
     shutdown</t>
   </si>
@@ -149,7 +149,7 @@
   </si>
   <si>
     <t xml:space="preserve">configure terminal
-  interface range {{ range }}
+  interface range {{ interface_range }}
     speed {{ speed }}
     duplex (( half or full ))</t>
   </si>
@@ -461,6 +461,382 @@
     <t xml:space="preserve">configure terminal
   line vty 0 {{ maximum }}
     ipv6 access-class {{ name }} (( in or out))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure dynamic ARP inspection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHCP snooping is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  ip arp inspection vlan {{ vlan_range }}
+  interface range {{ interface_range }}
+    ip arp inspection trust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure all additional validations for dynamic ARP inspection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic ARP inspection is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  ip arp inspection validate {{ src-mac }}
+  ip arp inspection validate {{ dst-mac }}
+  ip arp inspection validate {{ ip }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a rate limit for ARP packages on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    ip arp inspection limit rate {{ packets_per_second }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically recover an error disabled interface after a set period of time if the cause was ARP inspection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  errdisable recovery interval {{ seconds }}
+  errdisable recovery cause arp-inspection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manually set the time and date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clock set {{ hh }}:{{ mm }}:{{ ss }} {{ month }} {{ day }} {{ year }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure DHCP snooping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The DHCP option 72 should not be set to increase compatibility.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  ip dhcp snooping
+  ip dhcp snooping vlan {{ vlan_range }}
+  no ip dhcp snooping information option
+  interface range {{ interface_range }}
+    ip dhcp snooping trust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a rate limit for DHCP packages on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    ip dhcp snooping limit rate {{ packets_per_second }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically recover an error disabled interface after a set period of time if the cause was a DHCP rate limit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  errdisable recovery interval {{ seconds }}
+  errdisable recovery cause dhcp-rate-limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure port security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  switchport port-security max {{ number }}
+  switchport port-security mac (( sticky or {{ mac }} ))
+  switchport port-security violation (( protect or restrict or shutdown ))
+  switchport port-security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically recover an error disabled interface after a set period of time if the cause was port security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  errdisable recovery interval {{ seconds }}
+  errdisable recovery cause psecure-violation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a port channel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The LACP protocol should be used to facilitate this task.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface range {{ interface_range }}
+    channel-group {{ number }} mode (( active or passive ))
+  interface port-channel {{ number }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PAGP protocol should be used to facilitate this task.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface range {{ interface_range }}
+    channel-group {{ number }} mode (( desirable or auto ))
+  interface port-channel {{ number }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dynamic protocol should be used to facilitate this task.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface range {{ interface_range }}
+    channel-group {{ number }} mode on
+  interface port-channel {{ number }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure port channel load balancing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The port channel is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  port-channel load-balance (( src-mac or dst-mac or src-dst-mac or src-ip or dst-ip or src-dst-ip ))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure which spanning tree mode to use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  spanning-tree mode (( pvst or rapid-pvst or mst ))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure the spanning tree priority.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spanning tree is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  spanning-tree vlan {{ number }} priority {{ number }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure the spanning tree port priority of one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree vlan {{ number }} port-priority {{ number }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree BPDU guard on all portfast edge interfaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+    spanning-tree portfast edge bpduguard default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree portfast edge on all access ports.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+    spanning-tree portfast edge default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree loop guard on all interfaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+    spanning-tree loopguard default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree BPDU guard on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree bpduguard enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree portfast edge on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree portfast edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree loop guard on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree loopguard enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree uplinkfast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+    spanning-tree uplinkfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree backbonefast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+    spanning-tree backbonefast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree BPDU filter on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree bpdufilter enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spanning tree root guard on one interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    spanning-tree guard root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically recover an error disabled interface after a set period of time if the cause was BPDU guard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  errdisable recovery interval {{ seconds }}
+  errdisable recovery cause bpdu-guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and name a VLAN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vlan {{ number }}
+    name {{ name }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a VTPv2 server.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLANs area already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp domain {{ name }}
+  vtp version 2
+  vtp mode server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a VTPv2 client.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp domain {{ name }}
+  vtp version 2
+  vtp mode client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure authentication for VTPv2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTPv2 is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp password {{ password }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure VTP for automatic pruning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTP is already set up for basic operation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp pruning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a primary VTPv3 server.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp domain {{ name }}
+  vtp version 3
+  vtp mode server
+  end
+vtp primary force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a secondary VTPv3 server.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp domain {{ name }}
+  vtp version 3
+  vtp mode server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a VTPv3 client.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp domain {{ name }}
+  vtp version 3
+  vtp mode client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure authentication for VTPv3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTPv3 is already set up for basic operation.
+The password should not be stored as plain text in the VLAN database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  vtp password {{ password }} hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure the OSPFv2 network type of an interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    ip ospf network {{ 'broadcast' or 'non-broadcast' or 'point-to-point' or 'point-to-multipoint' or 'point-to-multipoint non-broadcast' }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure the OSPFv2 priority of an interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    ip ospf priority {{ priority }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure OSPFv2 to advertise a default route.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSPFv2 is already set up for basic operation.
+The route should be advertised even if no default route is present in the routing table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  router ospf {{ number }}
+    default-information originate always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure a trunk port.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No DTP negotiation should take place.
+802.1Q should be used for VLAN encapsulation.
+The allowed VLANs should be set explicitly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure terminal
+  interface {{ interface }}
+    switchport trunk encapsulation dot1q
+    switchport trunk native vlan {{ VLAN }}
+    switchport trunk allowed vlan {{ VLAN }}
+    switchport mode trunk
+    switchport nonegotiate</t>
   </si>
 </sst>
 </file>
@@ -548,7 +924,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,6 +939,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -642,10 +1022,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -654,7 +1034,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="90.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="92.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="72.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="79.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="54.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44.27"/>
@@ -755,7 +1135,7 @@
       <c r="J2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="0"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1259,6 +1639,544 @@
       </c>
       <c r="F38" s="3" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>